<commit_message>
new source data with pct of renter occupied at 100
</commit_message>
<xml_diff>
--- a/resources/housing_security/EDDT_UnitsAffordablebyAMI_2015-2019.xlsx
+++ b/resources/housing_security/EDDT_UnitsAffordablebyAMI_2015-2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nyco365-my.sharepoint.com/personal/emaurer_planning_nyc_gov/Documents/Attachments/EDDT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20EAF7DB-3012-491D-A278-97B5ADA15651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{BCBA3E02-C4A6-4AF9-8486-FA6E9B734CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB4E6D04-53AC-46C2-BC37-58B660E4AFAA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{973DDEAA-05DE-4504-8606-6550B349B5AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{973DDEAA-05DE-4504-8606-6550B349B5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="2" r:id="rId1"/>
@@ -267,7 +267,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,17 +727,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B7FF20-B102-4897-8D1D-4482A4CAB0FC}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -751,7 +751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -759,7 +759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -767,7 +767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -775,7 +775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -783,7 +783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>12</v>
       </c>
@@ -791,7 +791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
         <v>14</v>
       </c>
@@ -805,7 +805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
@@ -819,7 +819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
@@ -833,7 +833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
@@ -847,7 +847,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
@@ -861,7 +861,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
@@ -875,7 +875,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
@@ -889,7 +889,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>30</v>
       </c>
@@ -903,14 +903,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932BA79C-917E-483E-8764-5157FB418B69}">
   <dimension ref="A1:AJ62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>0.2</v>
       </c>
       <c r="E2" s="7">
-        <v>52.3</v>
+        <v>100</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>68</v>
@@ -1130,7 +1130,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0.4</v>
       </c>
       <c r="E3" s="11">
-        <v>68.5</v>
+        <v>100</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>68</v>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>0.3</v>
       </c>
       <c r="E4" s="11">
-        <v>54.6</v>
+        <v>100</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>68</v>
@@ -1350,7 +1350,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>0.5</v>
       </c>
       <c r="E5" s="11">
-        <v>63.7</v>
+        <v>100</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>68</v>
@@ -1460,7 +1460,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>0.5</v>
       </c>
       <c r="E6" s="11">
-        <v>37.700000000000003</v>
+        <v>100</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>68</v>
@@ -1570,7 +1570,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="11">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>68</v>
@@ -1680,7 +1680,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>3701</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>1.8</v>
       </c>
       <c r="E8" s="11">
-        <v>59.1</v>
+        <v>100</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>68</v>
@@ -1790,7 +1790,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>3702</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E9" s="11">
-        <v>46.1</v>
+        <v>100</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>68</v>
@@ -1900,7 +1900,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>3703</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>3.1</v>
       </c>
       <c r="E10" s="11">
-        <v>47.2</v>
+        <v>100</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>68</v>
@@ -2010,7 +2010,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>3704</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>1.9</v>
       </c>
       <c r="E11" s="11">
-        <v>54.7</v>
+        <v>100</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>68</v>
@@ -2120,7 +2120,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>3705</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="11">
-        <v>88.4</v>
+        <v>100</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>68</v>
@@ -2230,7 +2230,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>3706</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E13" s="11">
-        <v>72.400000000000006</v>
+        <v>100</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>68</v>
@@ -2340,7 +2340,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>3707</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0.9</v>
       </c>
       <c r="E14" s="11">
-        <v>81.5</v>
+        <v>100</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>68</v>
@@ -2450,7 +2450,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>3708</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="11">
-        <v>80.599999999999994</v>
+        <v>100</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>68</v>
@@ -2560,7 +2560,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>3709</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E16" s="11">
-        <v>67.599999999999994</v>
+        <v>100</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>68</v>
@@ -2670,7 +2670,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>3710</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="11">
-        <v>88.9</v>
+        <v>100</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>68</v>
@@ -2780,7 +2780,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>3801</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E18" s="11">
-        <v>62.5</v>
+        <v>100</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>68</v>
@@ -2890,7 +2890,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>3802</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>1.6</v>
       </c>
       <c r="E19" s="11">
-        <v>58.4</v>
+        <v>100</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>68</v>
@@ -3000,7 +3000,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>3803</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>1.4</v>
       </c>
       <c r="E20" s="11">
-        <v>75.2</v>
+        <v>100</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>68</v>
@@ -3110,7 +3110,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>3804</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E21" s="11">
-        <v>92.2</v>
+        <v>100</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>68</v>
@@ -3220,7 +3220,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>3805</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E22" s="11">
-        <v>55.3</v>
+        <v>100</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>68</v>
@@ -3330,7 +3330,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>3806</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="11">
-        <v>57.3</v>
+        <v>100</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>68</v>
@@ -3440,7 +3440,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>3807</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>1.4</v>
       </c>
       <c r="E24" s="11">
-        <v>65.7</v>
+        <v>100</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>68</v>
@@ -3550,7 +3550,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>3808</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>2.1</v>
       </c>
       <c r="E25" s="11">
-        <v>54.3</v>
+        <v>100</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>68</v>
@@ -3660,7 +3660,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>3809</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="11">
-        <v>86.7</v>
+        <v>100</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>68</v>
@@ -3770,7 +3770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>3810</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>1.9</v>
       </c>
       <c r="E27" s="11">
-        <v>53.8</v>
+        <v>100</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>68</v>
@@ -3880,7 +3880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>3901</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>6.4</v>
       </c>
       <c r="E28" s="11">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>68</v>
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>3902</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E29" s="11">
-        <v>21.1</v>
+        <v>100</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>68</v>
@@ -4100,7 +4100,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>3903</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>2.6</v>
       </c>
       <c r="E30" s="11">
-        <v>34.6</v>
+        <v>100</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>68</v>
@@ -4210,7 +4210,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>4001</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>1.2</v>
       </c>
       <c r="E31" s="11">
-        <v>62.8</v>
+        <v>100</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>68</v>
@@ -4320,7 +4320,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>4002</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>1.2</v>
       </c>
       <c r="E32" s="11">
-        <v>60.4</v>
+        <v>100</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>68</v>
@@ -4430,7 +4430,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>4003</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>1.6</v>
       </c>
       <c r="E33" s="11">
-        <v>59.5</v>
+        <v>100</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>68</v>
@@ -4540,7 +4540,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>4004</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>1.5</v>
       </c>
       <c r="E34" s="11">
-        <v>54.5</v>
+        <v>100</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>68</v>
@@ -4650,7 +4650,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>4005</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>2.1</v>
       </c>
       <c r="E35" s="11">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>68</v>
@@ -4760,7 +4760,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>4006</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>1.4</v>
       </c>
       <c r="E36" s="11">
-        <v>63.9</v>
+        <v>100</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>68</v>
@@ -4870,7 +4870,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>4007</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>1.5</v>
       </c>
       <c r="E37" s="11">
-        <v>88.2</v>
+        <v>100</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>68</v>
@@ -4980,7 +4980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>4008</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>1.7</v>
       </c>
       <c r="E38" s="11">
-        <v>65.2</v>
+        <v>100</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>68</v>
@@ -5090,7 +5090,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>4009</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E39" s="11">
-        <v>29.3</v>
+        <v>100</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>68</v>
@@ -5200,7 +5200,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="40" spans="1:36">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>4010</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>1.9</v>
       </c>
       <c r="E40" s="11">
-        <v>49.1</v>
+        <v>100</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>68</v>
@@ -5310,7 +5310,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>4011</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>1.3</v>
       </c>
       <c r="E41" s="11">
-        <v>65.900000000000006</v>
+        <v>100</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>68</v>
@@ -5420,7 +5420,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>4012</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>1.8</v>
       </c>
       <c r="E42" s="11">
-        <v>47.2</v>
+        <v>100</v>
       </c>
       <c r="F42" s="12" t="s">
         <v>68</v>
@@ -5530,7 +5530,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="43" spans="1:36">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>4013</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>1.9</v>
       </c>
       <c r="E43" s="11">
-        <v>46.3</v>
+        <v>100</v>
       </c>
       <c r="F43" s="12" t="s">
         <v>68</v>
@@ -5640,7 +5640,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>4014</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="11">
-        <v>50.2</v>
+        <v>100</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>68</v>
@@ -5750,7 +5750,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>4015</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>1.3</v>
       </c>
       <c r="E45" s="11">
-        <v>60.5</v>
+        <v>100</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>68</v>
@@ -5860,7 +5860,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>4016</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E46" s="11">
-        <v>43.4</v>
+        <v>100</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>68</v>
@@ -5970,7 +5970,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>4017</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>1.6</v>
       </c>
       <c r="E47" s="11">
-        <v>45.5</v>
+        <v>100</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>68</v>
@@ -6080,7 +6080,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>4018</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>1.8</v>
       </c>
       <c r="E48" s="11">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>68</v>
@@ -6190,7 +6190,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>4101</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>1.4</v>
       </c>
       <c r="E49" s="11">
-        <v>62.8</v>
+        <v>100</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>68</v>
@@ -6300,7 +6300,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>4102</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>1.8</v>
       </c>
       <c r="E50" s="11">
-        <v>39.9</v>
+        <v>100</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>68</v>
@@ -6410,7 +6410,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>4103</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>1.8</v>
       </c>
       <c r="E51" s="11">
-        <v>38.5</v>
+        <v>100</v>
       </c>
       <c r="F51" s="12" t="s">
         <v>68</v>
@@ -6520,7 +6520,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>4104</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>3.6</v>
       </c>
       <c r="E52" s="11">
-        <v>21.4</v>
+        <v>100</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>68</v>
@@ -6630,7 +6630,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>4105</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>3.8</v>
       </c>
       <c r="E53" s="11">
-        <v>15.8</v>
+        <v>100</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>68</v>
@@ -6740,7 +6740,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>4106</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E54" s="11">
-        <v>38.5</v>
+        <v>100</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>68</v>
@@ -6850,7 +6850,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="55" spans="1:36">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>4107</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>1.6</v>
       </c>
       <c r="E55" s="11">
-        <v>46.1</v>
+        <v>100</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>68</v>
@@ -6960,7 +6960,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>4108</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>2.7</v>
       </c>
       <c r="E56" s="11">
-        <v>45.9</v>
+        <v>100</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>68</v>
@@ -7070,7 +7070,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>4109</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>1.6</v>
       </c>
       <c r="E57" s="11">
-        <v>49.6</v>
+        <v>100</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>68</v>
@@ -7180,7 +7180,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>4110</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>1.8</v>
       </c>
       <c r="E58" s="11">
-        <v>38.6</v>
+        <v>100</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>68</v>
@@ -7290,7 +7290,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>4111</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>2.1</v>
       </c>
       <c r="E59" s="11">
-        <v>31.9</v>
+        <v>100</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>68</v>
@@ -7400,7 +7400,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>4112</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>2.1</v>
       </c>
       <c r="E60" s="11">
-        <v>31.9</v>
+        <v>100</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>68</v>
@@ -7510,7 +7510,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>4113</v>
       </c>
@@ -7524,7 +7524,7 @@
         <v>3.4</v>
       </c>
       <c r="E61" s="11">
-        <v>18.899999999999999</v>
+        <v>100</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>68</v>
@@ -7620,7 +7620,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>4114</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E62" s="11">
-        <v>52.6</v>
+        <v>100</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>68</v>
@@ -7960,13 +7960,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E133EB11-0637-4D8E-B8A0-3C93C1C213EF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E133EB11-0637-4D8E-B8A0-3C93C1C213EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a006254a-362b-4ff4-965e-371f488d1924"/>
+    <ds:schemaRef ds:uri="0974b3c8-8b09-43c3-8cba-9a7da3221e79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3732304-1B6D-44A6-8FBC-2D2C08F82783}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3732304-1B6D-44A6-8FBC-2D2C08F82783}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369535BA-2715-45BD-BA56-047FAF28A8FD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369535BA-2715-45BD-BA56-047FAF28A8FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0974b3c8-8b09-43c3-8cba-9a7da3221e79"/>
+    <ds:schemaRef ds:uri="a006254a-362b-4ff4-965e-371f488d1924"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>